<commit_message>
Adding edited scraper outputs
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2021-02-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2021-02-22.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwatkins/COVID19_tracker_data_extraction/workflow/python/output/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E714C80-93E4-E14E-ABC5-E119C5FABF18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="14120" yWindow="920" windowWidth="28880" windowHeight="18340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -271,12 +277,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +297,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -328,19 +346,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -387,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,9 +447,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,6 +499,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -628,14 +692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,27 +748,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="B2" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C2" s="4">
+        <v>766405</v>
+      </c>
+      <c r="D2" s="4">
+        <v>22858</v>
+      </c>
+      <c r="E2" s="4">
+        <v>60031</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3625</v>
+      </c>
+      <c r="G2" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>16.27</v>
+      </c>
+      <c r="I2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4">
         <v>1196764</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>13.47</v>
       </c>
       <c r="O2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -743,27 +832,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="B4" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C4" s="4">
+        <v>424176</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9466</v>
+      </c>
+      <c r="E4" s="4">
+        <v>133455</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3637</v>
+      </c>
+      <c r="G4" s="4">
+        <v>31.46</v>
+      </c>
+      <c r="H4" s="4">
+        <v>38.42</v>
+      </c>
+      <c r="I4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4">
         <v>1502916</v>
       </c>
-      <c r="N4">
-        <v>32.23</v>
+      <c r="N4" s="4">
+        <v>32.229999999999997</v>
       </c>
       <c r="O4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -810,27 +922,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6">
+      <c r="B6" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C6" s="4">
+        <v>844770</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10934</v>
+      </c>
+      <c r="E6" s="4">
+        <v>141498</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2550</v>
+      </c>
+      <c r="G6" s="4">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4">
         <v>2179622</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>21.46</v>
       </c>
       <c r="O6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -877,7 +1012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -909,7 +1044,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -956,7 +1091,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -979,7 +1114,7 @@
         <v>2.95</v>
       </c>
       <c r="H10">
-        <v>2.43</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -1003,7 +1138,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1050,21 +1185,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
+      <c r="B12" s="2">
+        <v>44246</v>
+      </c>
+      <c r="C12" s="4">
+        <v>504149</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8324</v>
+      </c>
+      <c r="E12" s="4">
+        <v>103049</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2278</v>
+      </c>
+      <c r="G12" s="4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>27.4</v>
+      </c>
+      <c r="I12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="4">
+        <v>1390153</v>
+      </c>
+      <c r="N12" s="4">
+        <v>27</v>
       </c>
       <c r="O12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1087,7 +1251,7 @@
         <v>12.76</v>
       </c>
       <c r="H13">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -1105,27 +1269,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="B14" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C14" s="4">
+        <v>43594</v>
+      </c>
+      <c r="D14" s="4">
+        <v>658</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2197</v>
+      </c>
+      <c r="F14" s="4">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="4">
         <v>17881</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>1.34</v>
       </c>
       <c r="O14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1172,7 +1359,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1406,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1266,7 +1453,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1313,7 +1500,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1541,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1395,87 +1582,179 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="B21" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C21" s="4">
+        <v>22787</v>
+      </c>
+      <c r="D21" s="4">
+        <v>406</v>
+      </c>
+      <c r="E21" s="4">
+        <v>560</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="4">
         <v>26266</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <v>1.85</v>
       </c>
       <c r="O21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22">
+      <c r="B22" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C22" s="4">
+        <v>419853</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4203</v>
+      </c>
+      <c r="E22" s="4">
+        <v>22591</v>
+      </c>
+      <c r="F22" s="4">
+        <v>255</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5.38</v>
+      </c>
+      <c r="H22" s="4">
+        <v>6.07</v>
+      </c>
+      <c r="I22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="4">
         <v>287959</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="4">
         <v>7.35</v>
       </c>
       <c r="O22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="b">
-        <v>0</v>
-      </c>
-      <c r="M23">
+      <c r="B23" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C23" s="4">
+        <v>98810</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1341</v>
+      </c>
+      <c r="E23" s="4">
+        <v>451</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="4">
         <v>4630</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="4">
         <v>0.44</v>
       </c>
       <c r="O23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="I24" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="B24" s="2">
+        <v>44246</v>
+      </c>
+      <c r="C24" s="4">
+        <v>290832</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4614</v>
+      </c>
+      <c r="E24" s="4">
+        <v>14056</v>
+      </c>
+      <c r="F24" s="4">
+        <v>227</v>
+      </c>
+      <c r="G24" s="4">
+        <v>4.83</v>
+      </c>
+      <c r="H24" s="4">
+        <v>4.92</v>
+      </c>
+      <c r="I24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="4">
         <v>169801</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>5.84</v>
       </c>
       <c r="O24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1522,21 +1801,46 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="b">
-        <v>0</v>
+      <c r="B26" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C26" s="4">
+        <v>99312</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1438</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2845</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4">
+        <v>2.86</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="4">
+        <v>25911</v>
+      </c>
+      <c r="N26" s="4">
+        <v>3.4</v>
       </c>
       <c r="O26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1577,47 +1881,93 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="I28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J28" t="b">
-        <v>0</v>
-      </c>
-      <c r="M28">
+      <c r="B28" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C28" s="4">
+        <v>359584</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5374</v>
+      </c>
+      <c r="E28" s="4">
+        <v>10788</v>
+      </c>
+      <c r="F28" s="4">
+        <v>130</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2.42</v>
+      </c>
+      <c r="I28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="4">
         <v>109911</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>3.51</v>
       </c>
       <c r="O28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="I29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" t="b">
-        <v>0</v>
-      </c>
-      <c r="M29">
+      <c r="B29" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C29" s="4">
+        <v>475348</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7715</v>
+      </c>
+      <c r="E29" s="4">
+        <v>41356</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1011</v>
+      </c>
+      <c r="G29" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H29" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="I29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="4">
         <v>704896</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="4">
         <v>11.57</v>
       </c>
       <c r="O29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1658,27 +2008,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
-      <c r="I31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J31" t="b">
-        <v>0</v>
-      </c>
-      <c r="M31">
+      <c r="B31" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C31" s="4">
+        <v>290874</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6553</v>
+      </c>
+      <c r="E31" s="4">
+        <v>96147</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2589</v>
+      </c>
+      <c r="G31" s="4">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="H31" s="4">
+        <v>39.5</v>
+      </c>
+      <c r="I31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="4">
         <v>1125834</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="4">
         <v>37.67</v>
       </c>
       <c r="O31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1719,27 +2092,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
-      <c r="I33" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="M33">
+      <c r="B33" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C33" s="4">
+        <v>290972</v>
+      </c>
+      <c r="D33" s="4">
+        <v>4872</v>
+      </c>
+      <c r="E33" s="4">
+        <v>22114</v>
+      </c>
+      <c r="F33" s="4">
+        <v>453</v>
+      </c>
+      <c r="G33" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="H33" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="4">
         <v>261123</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="4">
         <v>8.93</v>
       </c>
       <c r="O33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1780,7 +2176,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1827,7 +2223,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1868,13 +2264,13 @@
         <v>90860</v>
       </c>
       <c r="N36">
-        <v>4.77</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="O36" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1894,7 +2290,7 @@
         <v>2972</v>
       </c>
       <c r="G37">
-        <v>4.06</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H37">
         <v>6.23</v>
@@ -1921,21 +2317,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="I38" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" t="b">
-        <v>0</v>
+      <c r="B38" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C38" s="4">
+        <v>111334</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1863</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2483</v>
+      </c>
+      <c r="F38" s="4">
+        <v>7</v>
+      </c>
+      <c r="G38" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="I38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="4">
+        <v>20348</v>
+      </c>
+      <c r="N38" s="4">
+        <v>2.2999999999999998</v>
       </c>
       <c r="O38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1982,7 +2407,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2017,7 +2442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2052,33 +2477,56 @@
         <v>3316376</v>
       </c>
       <c r="N41">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>55</v>
       </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="b">
-        <v>0</v>
-      </c>
-      <c r="M42">
+      <c r="B42" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C42" s="4">
+        <v>39755</v>
+      </c>
+      <c r="D42" s="4">
+        <v>995</v>
+      </c>
+      <c r="E42" s="4">
+        <v>19339</v>
+      </c>
+      <c r="F42" s="4">
+        <v>743</v>
+      </c>
+      <c r="G42" s="4">
+        <v>49</v>
+      </c>
+      <c r="H42" s="4">
+        <v>75</v>
+      </c>
+      <c r="I42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="4">
         <v>321317</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="4">
         <v>46.94</v>
       </c>
       <c r="O42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2125,47 +2573,93 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="I44" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" t="b">
-        <v>0</v>
-      </c>
-      <c r="M44">
+      <c r="B44" s="2">
+        <v>44247</v>
+      </c>
+      <c r="C44" s="4">
+        <v>169150</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1826</v>
+      </c>
+      <c r="E44" s="4">
+        <v>989</v>
+      </c>
+      <c r="F44" s="4">
+        <v>9</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="4">
         <v>11536</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="4">
         <v>0.68</v>
       </c>
       <c r="O44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="I45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" t="b">
-        <v>0</v>
-      </c>
-      <c r="M45">
+      <c r="B45" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C45" s="4">
+        <v>915018</v>
+      </c>
+      <c r="D45" s="4">
+        <v>23614</v>
+      </c>
+      <c r="E45" s="4">
+        <v>78019</v>
+      </c>
+      <c r="F45" s="4">
+        <v>2829</v>
+      </c>
+      <c r="G45" s="4">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="H45" s="4">
+        <v>11.98</v>
+      </c>
+      <c r="I45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="4">
         <v>1423319</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="4">
         <v>11.13</v>
       </c>
       <c r="O45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2206,13 +2700,13 @@
         <v>305259</v>
       </c>
       <c r="N46">
-        <v>4.39</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="O46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2253,7 +2747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2288,27 +2782,52 @@
         <v>1613285</v>
       </c>
       <c r="N48">
-        <v>19.17</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="O48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" t="b">
-        <v>0</v>
+      <c r="B49" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C49" s="4">
+        <v>129854</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2263</v>
+      </c>
+      <c r="E49" s="4">
+        <v>3390</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="4">
+        <v>2.61</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="4">
+        <v>64518</v>
+      </c>
+      <c r="N49" s="4">
+        <v>3.6</v>
       </c>
       <c r="O49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2349,40 +2868,86 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
-      <c r="I51" t="b">
-        <v>0</v>
-      </c>
-      <c r="J51" t="b">
-        <v>0</v>
-      </c>
-      <c r="M51">
+      <c r="B51" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C51" s="4">
+        <v>73413</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1154</v>
+      </c>
+      <c r="E51" s="4">
+        <v>973</v>
+      </c>
+      <c r="F51" s="4">
+        <v>12</v>
+      </c>
+      <c r="G51" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="H51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="4">
         <v>20516</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="4">
         <v>1.53</v>
       </c>
       <c r="O51" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
-      <c r="I52" t="b">
-        <v>0</v>
-      </c>
-      <c r="J52" t="b">
-        <v>0</v>
-      </c>
-      <c r="M52">
+      <c r="B52" s="2">
+        <v>44248</v>
+      </c>
+      <c r="C52" s="4">
+        <v>396997</v>
+      </c>
+      <c r="D52" s="4">
+        <v>4447</v>
+      </c>
+      <c r="E52" s="4">
+        <v>33666</v>
+      </c>
+      <c r="F52" s="4">
+        <v>372</v>
+      </c>
+      <c r="G52" s="4">
+        <v>8.48</v>
+      </c>
+      <c r="H52" s="4">
+        <v>8.36</v>
+      </c>
+      <c r="I52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="4">
         <v>354112</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="4">
         <v>7.98</v>
       </c>
       <c r="O52" t="s">

</xml_diff>